<commit_message>
Su2c files added, Vignette updated
</commit_message>
<xml_diff>
--- a/inst/extdata/grnsumm.xlsx
+++ b/inst/extdata/grnsumm.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t xml:space="preserve">Drivers</t>
   </si>
@@ -30,142 +30,289 @@
     <t xml:space="preserve">XOR</t>
   </si>
   <si>
-    <t xml:space="preserve">BATF2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BCL2L15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HRASLS2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KCNJ16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REG1A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SFTA2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USH1C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FOXA3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANXA13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARL14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHRNA7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FOLR1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IGF2BP3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LPCAT4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCSK9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLA2G10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PPP1R14D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SLC13A2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSX1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAX6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANKS4B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APOBEC1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATP10B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C20orf202</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C6orf222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CASP5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CEACAM7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EVPLL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HHLA2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HKDC1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KRT84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUC17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMUR2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTPRH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SYNGR4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRIM15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UGT1A8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOX5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OASL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUT3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CA9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MST1R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ONECUT3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUT2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOS2</t>
+    <t xml:space="preserve">ARID4B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXOC3L1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCL6B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACVRL1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADAMTS7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALPK3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APLN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APLNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APOLD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARHGEF15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BDKRB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDH5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLEC14A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLEC1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COX4I2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CXorf36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CYYR1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DLL4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FGD5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GABRD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIPC3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GJC1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPR4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPRC5B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIGD1B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSPA12B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LZTS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMRN2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MYCT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOVA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OLFML2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCDH12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCDH17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDGFB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLVAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLXDC1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTPRB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAMP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RASL12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGS5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RHOJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROBO4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPRY4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STARD8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TBXA2R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THSD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THY1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIE1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMEM233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TNFAIP8L1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VASH1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELK3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECSCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GGT5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GJA4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KCNJ8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LGMN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LHFP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDGFD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PECAM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAMP3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOXS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BGN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLDN5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FJX1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FNDC1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTRA3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IGFBP7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KANK3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LRRC32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OLFML2B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RASIP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLIT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMEM204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C11orf24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHST1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDNRB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KDELC1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAMP5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMP11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGS3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPPP3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGFL7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLA2G15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEMA6B</t>
   </si>
   <si>
     <t xml:space="preserve"/>
@@ -177,13 +324,10 @@
     <t xml:space="preserve">Cliques</t>
   </si>
   <si>
-    <t xml:space="preserve">GATA4,HNF4A,NR1H4,PAX6,DMRT1,DMRT2,NKX3-1,FEZF1,HAND2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISX,E2F7,NR0B2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FOXA3,GATA4,HNF4A,NR1H4,DMRT1,DMRT2,NKX3-1,FEZF1,HAND2</t>
+    <t xml:space="preserve">EBF1,ELK3,ETS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCL6B,EBF1,ETS1</t>
   </si>
 </sst>
 </file>
@@ -551,10 +695,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -568,10 +712,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -585,10 +729,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -602,27 +746,27 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
@@ -636,7 +780,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -653,7 +797,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -662,15 +806,15 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -679,15 +823,15 @@
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -696,15 +840,15 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
@@ -713,15 +857,15 @@
         <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
@@ -738,7 +882,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>19</v>
@@ -747,15 +891,15 @@
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
@@ -764,15 +908,15 @@
         <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
@@ -781,52 +925,52 @@
         <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C17" t="n">
         <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C18" t="n">
         <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C19" t="n">
         <v>1</v>
@@ -840,10 +984,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" t="n">
         <v>1</v>
@@ -857,10 +1001,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C21" t="n">
         <v>1</v>
@@ -874,112 +1018,112 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C22" t="n">
         <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C23" t="n">
         <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C24" t="n">
         <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C25" t="n">
         <v>1</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C26" t="n">
         <v>1</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C27" t="n">
         <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C28" t="n">
         <v>1</v>
@@ -993,10 +1137,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C29" t="n">
         <v>1</v>
@@ -1010,27 +1154,27 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C30" t="n">
         <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C31" t="n">
         <v>1</v>
@@ -1044,44 +1188,44 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C32" t="n">
         <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C33" t="n">
         <v>1</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C34" t="n">
         <v>1</v>
@@ -1095,27 +1239,27 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C35" t="n">
         <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C36" t="n">
         <v>1</v>
@@ -1129,112 +1273,112 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="C37" t="n">
         <v>1</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C38" t="n">
         <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C39" t="n">
         <v>1</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C40" t="n">
         <v>1</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C41" t="n">
         <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C42" t="n">
         <v>1</v>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C43" t="n">
         <v>1</v>
@@ -1248,10 +1392,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="C44" t="n">
         <v>1</v>
@@ -1265,10 +1409,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C45" t="n">
         <v>1</v>
@@ -1282,44 +1426,44 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C46" t="n">
         <v>1</v>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C47" t="n">
         <v>1</v>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="C48" t="n">
         <v>1</v>
@@ -1333,50 +1477,50 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="C49" t="n">
         <v>1</v>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="C50" t="n">
         <v>1</v>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51" t="n">
         <v>1</v>
@@ -1384,16 +1528,16 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E52" t="n">
         <v>1</v>
@@ -1401,84 +1545,84 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" t="n">
         <v>1</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B54" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54" t="n">
         <v>1</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B55" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55" t="n">
         <v>1</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B56" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56" t="n">
         <v>1</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57" t="n">
         <v>1</v>
@@ -1486,50 +1630,50 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B58" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58" t="n">
         <v>1</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B59" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59" t="n">
         <v>1</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60" t="n">
         <v>1</v>
@@ -1537,16 +1681,16 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E61" t="n">
         <v>1</v>
@@ -1554,16 +1698,16 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E62" t="n">
         <v>1</v>
@@ -1571,16 +1715,16 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E63" t="n">
         <v>1</v>
@@ -1588,16 +1732,16 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64" t="n">
         <v>1</v>
@@ -1605,16 +1749,16 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65" t="n">
         <v>1</v>
@@ -1622,16 +1766,16 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66" t="n">
         <v>1</v>
@@ -1639,16 +1783,16 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B67" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67" t="n">
         <v>1</v>
@@ -1656,33 +1800,33 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="B68" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68" t="n">
         <v>1</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="B69" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69" t="n">
         <v>1</v>
@@ -1690,16 +1834,16 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="B70" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70" t="n">
         <v>1</v>
@@ -1707,18 +1851,1208 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="B71" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E71" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>64</v>
+      </c>
+      <c r="B72" t="s">
+        <v>70</v>
+      </c>
+      <c r="C72" t="n">
+        <v>1</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>64</v>
+      </c>
+      <c r="B73" t="s">
+        <v>39</v>
+      </c>
+      <c r="C73" t="n">
+        <v>1</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>64</v>
+      </c>
+      <c r="B74" t="s">
+        <v>71</v>
+      </c>
+      <c r="C74" t="n">
+        <v>1</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>64</v>
+      </c>
+      <c r="B75" t="s">
+        <v>72</v>
+      </c>
+      <c r="C75" t="n">
+        <v>1</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>64</v>
+      </c>
+      <c r="B76" t="s">
+        <v>73</v>
+      </c>
+      <c r="C76" t="n">
+        <v>1</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>64</v>
+      </c>
+      <c r="B77" t="s">
+        <v>56</v>
+      </c>
+      <c r="C77" t="n">
+        <v>1</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>64</v>
+      </c>
+      <c r="B78" t="s">
+        <v>74</v>
+      </c>
+      <c r="C78" t="n">
+        <v>1</v>
+      </c>
+      <c r="D78" t="n">
+        <v>1</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>64</v>
+      </c>
+      <c r="B79" t="s">
+        <v>60</v>
+      </c>
+      <c r="C79" t="n">
+        <v>1</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>64</v>
+      </c>
+      <c r="B80" t="s">
+        <v>62</v>
+      </c>
+      <c r="C80" t="n">
+        <v>1</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>75</v>
+      </c>
+      <c r="B81" t="s">
+        <v>13</v>
+      </c>
+      <c r="C81" t="n">
+        <v>1</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0</v>
+      </c>
+      <c r="E81" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>75</v>
+      </c>
+      <c r="B82" t="s">
+        <v>76</v>
+      </c>
+      <c r="C82" t="n">
+        <v>1</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0</v>
+      </c>
+      <c r="E82" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>75</v>
+      </c>
+      <c r="B83" t="s">
+        <v>77</v>
+      </c>
+      <c r="C83" t="n">
+        <v>1</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>75</v>
+      </c>
+      <c r="B84" t="s">
+        <v>17</v>
+      </c>
+      <c r="C84" t="n">
+        <v>1</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>75</v>
+      </c>
+      <c r="B85" t="s">
+        <v>65</v>
+      </c>
+      <c r="C85" t="n">
+        <v>1</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>75</v>
+      </c>
+      <c r="B86" t="s">
+        <v>23</v>
+      </c>
+      <c r="C86" t="n">
+        <v>1</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>75</v>
+      </c>
+      <c r="B87" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" t="n">
+        <v>1</v>
+      </c>
+      <c r="D87" t="n">
+        <v>1</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>75</v>
+      </c>
+      <c r="B88" t="s">
+        <v>78</v>
+      </c>
+      <c r="C88" t="n">
+        <v>1</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0</v>
+      </c>
+      <c r="E88" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>75</v>
+      </c>
+      <c r="B89" t="s">
+        <v>79</v>
+      </c>
+      <c r="C89" t="n">
+        <v>1</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0</v>
+      </c>
+      <c r="E89" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>75</v>
+      </c>
+      <c r="B90" t="s">
+        <v>66</v>
+      </c>
+      <c r="C90" t="n">
+        <v>1</v>
+      </c>
+      <c r="D90" t="n">
+        <v>1</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>75</v>
+      </c>
+      <c r="B91" t="s">
+        <v>67</v>
+      </c>
+      <c r="C91" t="n">
+        <v>1</v>
+      </c>
+      <c r="D91" t="n">
+        <v>1</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>75</v>
+      </c>
+      <c r="B92" t="s">
+        <v>30</v>
+      </c>
+      <c r="C92" t="n">
+        <v>1</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>75</v>
+      </c>
+      <c r="B93" t="s">
+        <v>35</v>
+      </c>
+      <c r="C93" t="n">
+        <v>1</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0</v>
+      </c>
+      <c r="E93" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>75</v>
+      </c>
+      <c r="B94" t="s">
+        <v>80</v>
+      </c>
+      <c r="C94" t="n">
+        <v>1</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0</v>
+      </c>
+      <c r="E94" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>75</v>
+      </c>
+      <c r="B95" t="s">
+        <v>81</v>
+      </c>
+      <c r="C95" t="n">
+        <v>1</v>
+      </c>
+      <c r="D95" t="n">
+        <v>1</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>75</v>
+      </c>
+      <c r="B96" t="s">
+        <v>82</v>
+      </c>
+      <c r="C96" t="n">
+        <v>1</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0</v>
+      </c>
+      <c r="E96" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>75</v>
+      </c>
+      <c r="B97" t="s">
+        <v>70</v>
+      </c>
+      <c r="C97" t="n">
+        <v>1</v>
+      </c>
+      <c r="D97" t="n">
+        <v>1</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>75</v>
+      </c>
+      <c r="B98" t="s">
+        <v>83</v>
+      </c>
+      <c r="C98" t="n">
+        <v>1</v>
+      </c>
+      <c r="D98" t="n">
+        <v>1</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>75</v>
+      </c>
+      <c r="B99" t="s">
+        <v>84</v>
+      </c>
+      <c r="C99" t="n">
+        <v>1</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0</v>
+      </c>
+      <c r="E99" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>75</v>
+      </c>
+      <c r="B100" t="s">
+        <v>73</v>
+      </c>
+      <c r="C100" t="n">
+        <v>1</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0</v>
+      </c>
+      <c r="E100" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>75</v>
+      </c>
+      <c r="B101" t="s">
+        <v>85</v>
+      </c>
+      <c r="C101" t="n">
+        <v>1</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0</v>
+      </c>
+      <c r="E101" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>75</v>
+      </c>
+      <c r="B102" t="s">
+        <v>51</v>
+      </c>
+      <c r="C102" t="n">
+        <v>1</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0</v>
+      </c>
+      <c r="E102" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>75</v>
+      </c>
+      <c r="B103" t="s">
+        <v>53</v>
+      </c>
+      <c r="C103" t="n">
+        <v>1</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0</v>
+      </c>
+      <c r="E103" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>75</v>
+      </c>
+      <c r="B104" t="s">
+        <v>86</v>
+      </c>
+      <c r="C104" t="n">
+        <v>1</v>
+      </c>
+      <c r="D104" t="n">
+        <v>1</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>75</v>
+      </c>
+      <c r="B105" t="s">
+        <v>60</v>
+      </c>
+      <c r="C105" t="n">
+        <v>1</v>
+      </c>
+      <c r="D105" t="n">
+        <v>0</v>
+      </c>
+      <c r="E105" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>75</v>
+      </c>
+      <c r="B106" t="s">
+        <v>87</v>
+      </c>
+      <c r="C106" t="n">
+        <v>1</v>
+      </c>
+      <c r="D106" t="n">
+        <v>0</v>
+      </c>
+      <c r="E106" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>5</v>
+      </c>
+      <c r="B107" t="s">
+        <v>88</v>
+      </c>
+      <c r="C107" t="n">
+        <v>0</v>
+      </c>
+      <c r="D107" t="n">
+        <v>1</v>
+      </c>
+      <c r="E107" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>5</v>
+      </c>
+      <c r="B108" t="s">
+        <v>20</v>
+      </c>
+      <c r="C108" t="n">
+        <v>0</v>
+      </c>
+      <c r="D108" t="n">
+        <v>1</v>
+      </c>
+      <c r="E108" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>5</v>
+      </c>
+      <c r="B109" t="s">
+        <v>30</v>
+      </c>
+      <c r="C109" t="n">
+        <v>0</v>
+      </c>
+      <c r="D109" t="n">
+        <v>1</v>
+      </c>
+      <c r="E109" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>7</v>
+      </c>
+      <c r="B110" t="s">
+        <v>76</v>
+      </c>
+      <c r="C110" t="n">
+        <v>0</v>
+      </c>
+      <c r="D110" t="n">
+        <v>1</v>
+      </c>
+      <c r="E110" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>7</v>
+      </c>
+      <c r="B111" t="s">
+        <v>89</v>
+      </c>
+      <c r="C111" t="n">
+        <v>0</v>
+      </c>
+      <c r="D111" t="n">
+        <v>1</v>
+      </c>
+      <c r="E111" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>7</v>
+      </c>
+      <c r="B112" t="s">
+        <v>65</v>
+      </c>
+      <c r="C112" t="n">
+        <v>0</v>
+      </c>
+      <c r="D112" t="n">
+        <v>1</v>
+      </c>
+      <c r="E112" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>7</v>
+      </c>
+      <c r="B113" t="s">
+        <v>90</v>
+      </c>
+      <c r="C113" t="n">
+        <v>0</v>
+      </c>
+      <c r="D113" t="n">
+        <v>1</v>
+      </c>
+      <c r="E113" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>7</v>
+      </c>
+      <c r="B114" t="s">
+        <v>66</v>
+      </c>
+      <c r="C114" t="n">
+        <v>0</v>
+      </c>
+      <c r="D114" t="n">
+        <v>1</v>
+      </c>
+      <c r="E114" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>7</v>
+      </c>
+      <c r="B115" t="s">
+        <v>68</v>
+      </c>
+      <c r="C115" t="n">
+        <v>0</v>
+      </c>
+      <c r="D115" t="n">
+        <v>1</v>
+      </c>
+      <c r="E115" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>7</v>
+      </c>
+      <c r="B116" t="s">
+        <v>91</v>
+      </c>
+      <c r="C116" t="n">
+        <v>0</v>
+      </c>
+      <c r="D116" t="n">
+        <v>1</v>
+      </c>
+      <c r="E116" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>7</v>
+      </c>
+      <c r="B117" t="s">
+        <v>92</v>
+      </c>
+      <c r="C117" t="n">
+        <v>0</v>
+      </c>
+      <c r="D117" t="n">
+        <v>1</v>
+      </c>
+      <c r="E117" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>7</v>
+      </c>
+      <c r="B118" t="s">
+        <v>93</v>
+      </c>
+      <c r="C118" t="n">
+        <v>0</v>
+      </c>
+      <c r="D118" t="n">
+        <v>1</v>
+      </c>
+      <c r="E118" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>7</v>
+      </c>
+      <c r="B119" t="s">
+        <v>94</v>
+      </c>
+      <c r="C119" t="n">
+        <v>0</v>
+      </c>
+      <c r="D119" t="n">
+        <v>1</v>
+      </c>
+      <c r="E119" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>7</v>
+      </c>
+      <c r="B120" t="s">
+        <v>95</v>
+      </c>
+      <c r="C120" t="n">
+        <v>0</v>
+      </c>
+      <c r="D120" t="n">
+        <v>1</v>
+      </c>
+      <c r="E120" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>7</v>
+      </c>
+      <c r="B121" t="s">
+        <v>86</v>
+      </c>
+      <c r="C121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D121" t="n">
+        <v>1</v>
+      </c>
+      <c r="E121" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>7</v>
+      </c>
+      <c r="B122" t="s">
+        <v>96</v>
+      </c>
+      <c r="C122" t="n">
+        <v>0</v>
+      </c>
+      <c r="D122" t="n">
+        <v>1</v>
+      </c>
+      <c r="E122" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>64</v>
+      </c>
+      <c r="B123" t="s">
+        <v>8</v>
+      </c>
+      <c r="C123" t="n">
+        <v>0</v>
+      </c>
+      <c r="D123" t="n">
+        <v>1</v>
+      </c>
+      <c r="E123" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>64</v>
+      </c>
+      <c r="B124" t="s">
+        <v>18</v>
+      </c>
+      <c r="C124" t="n">
+        <v>0</v>
+      </c>
+      <c r="D124" t="n">
+        <v>1</v>
+      </c>
+      <c r="E124" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>64</v>
+      </c>
+      <c r="B125" t="s">
+        <v>20</v>
+      </c>
+      <c r="C125" t="n">
+        <v>0</v>
+      </c>
+      <c r="D125" t="n">
+        <v>1</v>
+      </c>
+      <c r="E125" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>64</v>
+      </c>
+      <c r="B126" t="s">
+        <v>24</v>
+      </c>
+      <c r="C126" t="n">
+        <v>0</v>
+      </c>
+      <c r="D126" t="n">
+        <v>1</v>
+      </c>
+      <c r="E126" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>64</v>
+      </c>
+      <c r="B127" t="s">
+        <v>25</v>
+      </c>
+      <c r="C127" t="n">
+        <v>0</v>
+      </c>
+      <c r="D127" t="n">
+        <v>1</v>
+      </c>
+      <c r="E127" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>64</v>
+      </c>
+      <c r="B128" t="s">
+        <v>38</v>
+      </c>
+      <c r="C128" t="n">
+        <v>0</v>
+      </c>
+      <c r="D128" t="n">
+        <v>1</v>
+      </c>
+      <c r="E128" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>64</v>
+      </c>
+      <c r="B129" t="s">
+        <v>40</v>
+      </c>
+      <c r="C129" t="n">
+        <v>0</v>
+      </c>
+      <c r="D129" t="n">
+        <v>1</v>
+      </c>
+      <c r="E129" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>64</v>
+      </c>
+      <c r="B130" t="s">
+        <v>86</v>
+      </c>
+      <c r="C130" t="n">
+        <v>0</v>
+      </c>
+      <c r="D130" t="n">
+        <v>1</v>
+      </c>
+      <c r="E130" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>75</v>
+      </c>
+      <c r="B131" t="s">
+        <v>16</v>
+      </c>
+      <c r="C131" t="n">
+        <v>0</v>
+      </c>
+      <c r="D131" t="n">
+        <v>1</v>
+      </c>
+      <c r="E131" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>75</v>
+      </c>
+      <c r="B132" t="s">
+        <v>20</v>
+      </c>
+      <c r="C132" t="n">
+        <v>0</v>
+      </c>
+      <c r="D132" t="n">
+        <v>1</v>
+      </c>
+      <c r="E132" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>75</v>
+      </c>
+      <c r="B133" t="s">
+        <v>97</v>
+      </c>
+      <c r="C133" t="n">
+        <v>0</v>
+      </c>
+      <c r="D133" t="n">
+        <v>1</v>
+      </c>
+      <c r="E133" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>75</v>
+      </c>
+      <c r="B134" t="s">
+        <v>25</v>
+      </c>
+      <c r="C134" t="n">
+        <v>0</v>
+      </c>
+      <c r="D134" t="n">
+        <v>1</v>
+      </c>
+      <c r="E134" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>75</v>
+      </c>
+      <c r="B135" t="s">
+        <v>68</v>
+      </c>
+      <c r="C135" t="n">
+        <v>0</v>
+      </c>
+      <c r="D135" t="n">
+        <v>1</v>
+      </c>
+      <c r="E135" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>75</v>
+      </c>
+      <c r="B136" t="s">
+        <v>38</v>
+      </c>
+      <c r="C136" t="n">
+        <v>0</v>
+      </c>
+      <c r="D136" t="n">
+        <v>1</v>
+      </c>
+      <c r="E136" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>75</v>
+      </c>
+      <c r="B137" t="s">
+        <v>98</v>
+      </c>
+      <c r="C137" t="n">
+        <v>0</v>
+      </c>
+      <c r="D137" t="n">
+        <v>1</v>
+      </c>
+      <c r="E137" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>75</v>
+      </c>
+      <c r="B138" t="s">
+        <v>46</v>
+      </c>
+      <c r="C138" t="n">
+        <v>0</v>
+      </c>
+      <c r="D138" t="n">
+        <v>1</v>
+      </c>
+      <c r="E138" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>75</v>
+      </c>
+      <c r="B139" t="s">
+        <v>99</v>
+      </c>
+      <c r="C139" t="n">
+        <v>0</v>
+      </c>
+      <c r="D139" t="n">
+        <v>1</v>
+      </c>
+      <c r="E139" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>75</v>
+      </c>
+      <c r="B140" t="s">
+        <v>74</v>
+      </c>
+      <c r="C140" t="n">
+        <v>0</v>
+      </c>
+      <c r="D140" t="n">
+        <v>1</v>
+      </c>
+      <c r="E140" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>75</v>
+      </c>
+      <c r="B141" t="s">
+        <v>96</v>
+      </c>
+      <c r="C141" t="n">
+        <v>0</v>
+      </c>
+      <c r="D141" t="n">
+        <v>1</v>
+      </c>
+      <c r="E141" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1738,13 +3072,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2">
@@ -1755,62 +3089,40 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0.49</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="B4" t="n">
-        <v>0.8</v>
+        <v>0.93</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0.81</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>